<commit_message>
Changes to python document
Former-commit-id: 3852df0669f4b2201d7252291ca19799d6132c86
</commit_message>
<xml_diff>
--- a/Classifications/Master_Classifications.xlsx
+++ b/Classifications/Master_Classifications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iowa-my.sharepoint.com/personal/cjskalla_uiowa_edu/Documents/Documents/aerobictextreview/Classifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1685" documentId="11_F25DC773A252ABDACC1048EAE15952625BDE58EE" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3F89C99F-1E8F-4582-A518-C2F8115AC676}"/>
+  <xr:revisionPtr revIDLastSave="1695" documentId="11_F25DC773A252ABDACC1048EAE15952625BDE58EE" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E7E0F524-B579-4460-8319-74630E37F848}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="990" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="body-based helpful" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="1245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="1245">
   <si>
     <t>Video</t>
   </si>
@@ -3896,7 +3896,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3913,12 +3913,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3977,7 +3971,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3998,12 +3992,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4310,8 +4298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F174"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -6606,7 +6594,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>803</v>
       </c>
@@ -6625,8 +6613,8 @@
   <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7278,7 +7266,7 @@
       <c r="F42" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="G42" s="10" t="s">
+      <c r="G42" s="3" t="s">
         <v>533</v>
       </c>
     </row>
@@ -7604,6 +7592,9 @@
       <c r="A70" t="s">
         <v>803</v>
       </c>
+      <c r="B70" s="3" t="s">
+        <v>901</v>
+      </c>
       <c r="D70" s="2" t="s">
         <v>1095</v>
       </c>
@@ -7702,7 +7693,7 @@
       <c r="A77" t="s">
         <v>803</v>
       </c>
-      <c r="D77" s="12" t="s">
+      <c r="D77" s="10" t="s">
         <v>1225</v>
       </c>
       <c r="E77" s="2" t="s">
@@ -7712,49 +7703,49 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>803</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D78" s="10" t="s">
         <v>1105</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>1090</v>
       </c>
-      <c r="G78" s="11" t="s">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="G78" s="2" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>803</v>
       </c>
-      <c r="D79" s="12" t="s">
+      <c r="D79" s="10" t="s">
         <v>1226</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>1086</v>
       </c>
-      <c r="G79" s="11" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="G79" s="2" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>803</v>
       </c>
-      <c r="D80" s="12" t="s">
+      <c r="D80" s="10" t="s">
         <v>1227</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>1083</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>1133</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>803</v>
       </c>
@@ -7762,10 +7753,10 @@
         <v>469</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>1134</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>803</v>
       </c>
@@ -7773,7 +7764,7 @@
         <v>469</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>1185</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7784,18 +7775,18 @@
         <v>1092</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>803</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>1083</v>
       </c>
-      <c r="G84" s="2" t="s">
-        <v>1229</v>
+      <c r="G84" s="3" t="s">
+        <v>1238</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7805,19 +7796,13 @@
       <c r="E85" s="2" t="s">
         <v>1083</v>
       </c>
-      <c r="G85" s="2" t="s">
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>803</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>1086</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>1238</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -8103,11 +8088,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C253B67-1483-4793-A187-43AA0BC4321E}">
-  <dimension ref="A1:G301"/>
+  <dimension ref="A1:G303"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D296" sqref="D296"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F212" sqref="F212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10778,28 +10763,28 @@
         <v>900</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>803</v>
       </c>
-      <c r="E216" s="11" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E216" s="2" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>803</v>
       </c>
       <c r="E217" s="2" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>803</v>
       </c>
       <c r="E218" s="2" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -10807,151 +10792,151 @@
         <v>803</v>
       </c>
       <c r="E219" s="2" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>803</v>
       </c>
       <c r="E220" s="2" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>803</v>
       </c>
       <c r="E221" s="2" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>803</v>
       </c>
       <c r="E222" s="2" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>803</v>
       </c>
       <c r="E223" s="2" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>803</v>
       </c>
       <c r="E224" s="2" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>803</v>
       </c>
       <c r="E225" s="2" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>803</v>
       </c>
       <c r="E226" s="2" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>803</v>
       </c>
       <c r="E227" s="2" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="228" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>803</v>
       </c>
       <c r="E228" s="2" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>803</v>
       </c>
       <c r="E229" s="2" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="230" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>803</v>
       </c>
       <c r="E230" s="2" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>803</v>
       </c>
       <c r="E231" s="2" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>803</v>
       </c>
       <c r="E232" s="2" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>803</v>
       </c>
       <c r="E233" s="2" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>803</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>803</v>
       </c>
       <c r="E235" s="2" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>803</v>
       </c>
       <c r="E236" s="2" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>803</v>
       </c>
       <c r="E237" s="2" t="s">
-        <v>952</v>
+        <v>955</v>
       </c>
     </row>
     <row r="238" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -10959,15 +10944,15 @@
         <v>803</v>
       </c>
       <c r="E238" s="2" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>803</v>
       </c>
       <c r="E239" s="2" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="240" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -10975,7 +10960,7 @@
         <v>803</v>
       </c>
       <c r="E240" s="2" t="s">
-        <v>959</v>
+        <v>962</v>
       </c>
     </row>
     <row r="241" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -10983,79 +10968,79 @@
         <v>803</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>803</v>
       </c>
       <c r="E242" s="2" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>803</v>
       </c>
       <c r="E243" s="2" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>803</v>
       </c>
       <c r="E244" s="2" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>803</v>
       </c>
       <c r="E245" s="2" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>803</v>
       </c>
       <c r="E246" s="2" t="s">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>803</v>
       </c>
       <c r="E247" s="2" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>803</v>
       </c>
       <c r="E248" s="2" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>803</v>
       </c>
       <c r="E249" s="2" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>803</v>
       </c>
       <c r="E250" s="2" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
     </row>
     <row r="251" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -11063,7 +11048,7 @@
         <v>803</v>
       </c>
       <c r="E251" s="2" t="s">
-        <v>991</v>
+        <v>994</v>
       </c>
     </row>
     <row r="252" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -11071,15 +11056,15 @@
         <v>803</v>
       </c>
       <c r="E252" s="2" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="253" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>803</v>
       </c>
       <c r="E253" s="2" t="s">
-        <v>995</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="254" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -11087,7 +11072,7 @@
         <v>803</v>
       </c>
       <c r="E254" s="2" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="255" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -11095,15 +11080,15 @@
         <v>803</v>
       </c>
       <c r="E255" s="2" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>803</v>
       </c>
       <c r="E256" s="2" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="257" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -11111,7 +11096,7 @@
         <v>803</v>
       </c>
       <c r="E257" s="2" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="258" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -11119,31 +11104,31 @@
         <v>803</v>
       </c>
       <c r="E258" s="2" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="259" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>803</v>
       </c>
       <c r="E259" s="2" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="260" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>803</v>
       </c>
       <c r="E260" s="2" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="261" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>803</v>
       </c>
       <c r="E261" s="2" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="262" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -11151,7 +11136,7 @@
         <v>803</v>
       </c>
       <c r="E262" s="2" t="s">
-        <v>1014</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="263" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -11159,63 +11144,63 @@
         <v>803</v>
       </c>
       <c r="E263" s="2" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="264" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>803</v>
       </c>
       <c r="E264" s="2" t="s">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="265" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>803</v>
       </c>
       <c r="E265" s="2" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="266" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>803</v>
       </c>
       <c r="E266" s="2" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="267" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>803</v>
       </c>
       <c r="E267" s="2" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>803</v>
       </c>
       <c r="E268" s="2" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="269" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>803</v>
       </c>
       <c r="E269" s="2" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="270" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>803</v>
       </c>
       <c r="E270" s="2" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="271" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -11223,63 +11208,63 @@
         <v>803</v>
       </c>
       <c r="E271" s="2" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="272" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>803</v>
       </c>
       <c r="E272" s="2" t="s">
-        <v>1032</v>
-      </c>
-    </row>
-    <row r="273" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>803</v>
       </c>
       <c r="E273" s="2" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="274" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>803</v>
       </c>
       <c r="E274" s="2" t="s">
-        <v>1034</v>
-      </c>
-    </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>803</v>
       </c>
       <c r="E275" s="2" t="s">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="276" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>803</v>
       </c>
       <c r="E276" s="2" t="s">
-        <v>1036</v>
-      </c>
-    </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>803</v>
       </c>
       <c r="E277" s="2" t="s">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="278" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>803</v>
       </c>
       <c r="E278" s="2" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="279" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -11287,23 +11272,23 @@
         <v>803</v>
       </c>
       <c r="E279" s="2" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="280" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>803</v>
       </c>
       <c r="E280" s="2" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="281" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>803</v>
       </c>
       <c r="E281" s="2" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="282" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -11311,7 +11296,7 @@
         <v>803</v>
       </c>
       <c r="E282" s="2" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="283" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -11319,95 +11304,95 @@
         <v>803</v>
       </c>
       <c r="E283" s="2" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="284" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>803</v>
       </c>
       <c r="E284" s="2" t="s">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="285" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>803</v>
       </c>
       <c r="E285" s="2" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="286" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>803</v>
       </c>
       <c r="E286" s="2" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="287" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>803</v>
       </c>
       <c r="E287" s="2" t="s">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="288" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>803</v>
       </c>
       <c r="E288" s="2" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="289" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>803</v>
       </c>
       <c r="E289" s="2" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="290" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>803</v>
       </c>
       <c r="E290" s="2" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="291" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>803</v>
       </c>
       <c r="E291" s="2" t="s">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="292" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>803</v>
       </c>
       <c r="E292" s="2" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="293" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>803</v>
       </c>
       <c r="E293" s="2" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>803</v>
       </c>
       <c r="E294" s="2" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="295" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -11415,47 +11400,47 @@
         <v>803</v>
       </c>
       <c r="E295" s="2" t="s">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="296" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>803</v>
       </c>
       <c r="E296" s="2" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="297" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>803</v>
       </c>
       <c r="E297" s="2" t="s">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>803</v>
       </c>
       <c r="E298" s="2" t="s">
-        <v>1058</v>
-      </c>
-    </row>
-    <row r="299" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>803</v>
       </c>
       <c r="E299" s="2" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="300" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>803</v>
       </c>
-      <c r="E300" s="2" t="s">
-        <v>1061</v>
+      <c r="E300" s="3" t="s">
+        <v>1065</v>
       </c>
     </row>
     <row r="301" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -11463,7 +11448,20 @@
         <v>803</v>
       </c>
       <c r="E301" s="3" t="s">
-        <v>1065</v>
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>803</v>
+      </c>
+      <c r="E302" s="3" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>803</v>
       </c>
     </row>
   </sheetData>
@@ -11471,7 +11469,7 @@
   <conditionalFormatting sqref="F150">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E219">
+  <conditionalFormatting sqref="E218">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>